<commit_message>
Adding Modified Excel Sheet
</commit_message>
<xml_diff>
--- a/Koushik Practice.xlsx
+++ b/Koushik Practice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9a703be7d6fffab/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9a703be7d6fffab/Documents/KOUSHIK'S FILES/GIT Practice/koushiks-practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1941" documentId="8_{0562B34A-4E6E-4158-A4DB-DD0578809598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87F97499-1EDD-4BE8-AC1E-53A6CD06969D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{E3B6967F-E7C6-4CBF-9846-3DC7D9FBC476}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3B6967F-E7C6-4CBF-9846-3DC7D9FBC476}"/>
   </bookViews>
   <sheets>
     <sheet name="koushik practice" sheetId="1" r:id="rId1"/>
@@ -1593,30 +1593,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1648,6 +1624,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7225,10 +7225,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{835AE7EF-2C95-45D0-9CC4-B26906E077AA}" name="Table1" displayName="Table1" ref="A69:F75" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A69:F75" xr:uid="{835AE7EF-2C95-45D0-9CC4-B26906E077AA}"/>
@@ -7611,8 +7607,8 @@
   </sheetPr>
   <dimension ref="A1:U254"/>
   <sheetViews>
-    <sheetView topLeftCell="H31" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47:U49"/>
+    <sheetView tabSelected="1" topLeftCell="E95" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7686,11 +7682,11 @@
       <c r="H4">
         <v>40</v>
       </c>
-      <c r="M4" s="86" t="s">
+      <c r="M4" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
       <c r="R4" s="1" t="s">
         <v>18</v>
       </c>
@@ -7708,9 +7704,9 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="M5" s="86"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
+      <c r="M5" s="97"/>
+      <c r="N5" s="97"/>
+      <c r="O5" s="97"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -7726,9 +7722,9 @@
         <f>H1+H2+H3+H4+H5+H6+H7+H8+H9+H10-500</f>
         <v>150</v>
       </c>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -7740,9 +7736,9 @@
       <c r="H7">
         <v>70</v>
       </c>
-      <c r="M7" s="86"/>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
       <c r="R7" s="2" t="s">
         <v>18</v>
       </c>
@@ -7948,14 +7944,14 @@
       <c r="D24" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="87" t="s">
+      <c r="F24" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="87"/>
-      <c r="J24" s="87" t="s">
+      <c r="G24" s="98"/>
+      <c r="J24" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="87"/>
+      <c r="K24" s="98"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
@@ -7979,14 +7975,14 @@
       <c r="H25" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="88" t="s">
+      <c r="J25" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="89"/>
-      <c r="L25" s="89"/>
-      <c r="M25" s="89"/>
-      <c r="N25" s="89"/>
-      <c r="O25" s="90"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="101"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
@@ -8011,14 +8007,14 @@
       <c r="H26" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="J26" s="94" t="s">
+      <c r="J26" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="K26" s="95"/>
-      <c r="L26" s="95"/>
-      <c r="M26" s="95"/>
-      <c r="N26" s="95"/>
-      <c r="O26" s="96"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="87"/>
+      <c r="N26" s="87"/>
+      <c r="O26" s="88"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
@@ -8044,7 +8040,7 @@
         <f>G27/$G$26</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="J27" s="97" t="s">
+      <c r="J27" s="89" t="s">
         <v>47</v>
       </c>
       <c r="K27" s="28"/>
@@ -8085,7 +8081,7 @@
         <f t="shared" ref="H28:H33" si="0">G28/$G$26</f>
         <v>0.78</v>
       </c>
-      <c r="J28" s="98"/>
+      <c r="J28" s="90"/>
       <c r="K28" s="28">
         <v>10</v>
       </c>
@@ -8130,7 +8126,7 @@
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
-      <c r="J29" s="98"/>
+      <c r="J29" s="90"/>
       <c r="K29" s="28">
         <v>20</v>
       </c>
@@ -8175,7 +8171,7 @@
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="J30" s="98"/>
+      <c r="J30" s="90"/>
       <c r="K30" s="28">
         <v>30</v>
       </c>
@@ -8207,7 +8203,7 @@
         <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
-      <c r="J31" s="99"/>
+      <c r="J31" s="91"/>
       <c r="K31" s="28">
         <v>40</v>
       </c>
@@ -8365,10 +8361,10 @@
       <c r="F40" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="J40" s="85" t="s">
+      <c r="J40" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="K40" s="85"/>
+      <c r="K40" s="96"/>
       <c r="N40" s="34" t="s">
         <v>83</v>
       </c>
@@ -8481,10 +8477,10 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="G45" s="100" t="s">
+      <c r="G45" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="100"/>
+      <c r="H45" s="92"/>
       <c r="J45" s="30" t="s">
         <v>77</v>
       </c>
@@ -8596,27 +8592,27 @@
         <v>73</v>
       </c>
       <c r="P49" s="32" t="str">
-        <f>IF(P48&gt;80,"DISTINCTION",IF(P48&lt;35,"FAIL","PASS"))</f>
+        <f t="shared" ref="P49:U49" si="4">IF(P48&gt;80,"DISTINCTION",IF(P48&lt;35,"FAIL","PASS"))</f>
         <v>PASS</v>
       </c>
       <c r="Q49" s="32" t="str">
-        <f>IF(Q48&gt;80,"DISTINCTION",IF(Q48&lt;35,"FAIL","PASS"))</f>
+        <f t="shared" si="4"/>
         <v>DISTINCTION</v>
       </c>
       <c r="R49" s="32" t="str">
-        <f>IF(R48&gt;80,"DISTINCTION",IF(R48&lt;35,"FAIL","PASS"))</f>
+        <f t="shared" si="4"/>
         <v>DISTINCTION</v>
       </c>
       <c r="S49" s="32" t="str">
-        <f>IF(S48&gt;80,"DISTINCTION",IF(S48&lt;35,"FAIL","PASS"))</f>
+        <f t="shared" si="4"/>
         <v>DISTINCTION</v>
       </c>
       <c r="T49" s="32" t="str">
-        <f>IF(T48&gt;80,"DISTINCTION",IF(T48&lt;35,"FAIL","PASS"))</f>
+        <f t="shared" si="4"/>
         <v>FAIL</v>
       </c>
       <c r="U49" s="32" t="str">
-        <f>IF(U48&gt;80,"DISTINCTION",IF(U48&lt;35,"FAIL","PASS"))</f>
+        <f t="shared" si="4"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -8626,14 +8622,14 @@
       </c>
       <c r="H50" s="31">
         <f ca="1">IF(L31&gt;M31,TODAY(),TODAY()+29)</f>
-        <v>45737</v>
+        <v>45740</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J51" s="84" t="s">
+      <c r="J51" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="K51" s="84"/>
+      <c r="K51" s="95"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J52" s="29" t="s">
@@ -8666,15 +8662,15 @@
         <v>89</v>
       </c>
       <c r="L54" s="35" t="str">
-        <f t="shared" ref="L54:L58" si="4">IF(AND(K54&gt;=0,K54&lt;35),"FAIL",IF(AND(K54&gt;=35,K54&lt;=60),"PASS",IF(AND(K54&lt;=100,K54&gt;45),"DISTINCTION","INVALID")))</f>
+        <f t="shared" ref="L54:L58" si="5">IF(AND(K54&gt;=0,K54&lt;35),"FAIL",IF(AND(K54&gt;=35,K54&lt;=60),"PASS",IF(AND(K54&lt;=100,K54&gt;45),"DISTINCTION","INVALID")))</f>
         <v>DISTINCTION</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" s="83" t="s">
+      <c r="A55" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="83"/>
+      <c r="B55" s="94"/>
       <c r="J55" s="30" t="s">
         <v>76</v>
       </c>
@@ -8682,7 +8678,7 @@
         <v>-12</v>
       </c>
       <c r="L55" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>INVALID</v>
       </c>
     </row>
@@ -8708,7 +8704,7 @@
         <v>95</v>
       </c>
       <c r="L56" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DISTINCTION</v>
       </c>
     </row>
@@ -8717,7 +8713,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="22" t="b">
-        <f t="shared" ref="B57:B59" si="5">NOT(A57)</f>
+        <f t="shared" ref="B57:B59" si="6">NOT(A57)</f>
         <v>1</v>
       </c>
       <c r="E57" t="e">
@@ -8734,7 +8730,7 @@
         <v>45</v>
       </c>
       <c r="L57" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>PASS</v>
       </c>
     </row>
@@ -8743,7 +8739,7 @@
         <v>0</v>
       </c>
       <c r="B58" s="22" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J58" s="30" t="s">
@@ -8753,7 +8749,7 @@
         <v>29</v>
       </c>
       <c r="L58" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -8762,7 +8758,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="22" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -8916,7 +8912,7 @@
         <v>0.87</v>
       </c>
       <c r="F91" s="22" t="str">
-        <f t="shared" ref="F91:F101" si="6">VLOOKUP(B91,REMARKS,5,0)</f>
+        <f t="shared" ref="F91:F101" si="7">VLOOKUP(B91,REMARKS,5,0)</f>
         <v>PASS</v>
       </c>
     </row>
@@ -8934,7 +8930,7 @@
         <v>0.86</v>
       </c>
       <c r="F92" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -8952,7 +8948,7 @@
         <v>0.85</v>
       </c>
       <c r="F93" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>PASS</v>
       </c>
     </row>
@@ -8970,18 +8966,18 @@
         <v>0.93</v>
       </c>
       <c r="F94" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FAIL</v>
       </c>
       <c r="G94" t="s">
         <v>114</v>
       </c>
-      <c r="H94" s="101">
+      <c r="H94" s="93">
         <f>VLOOKUP(G94,C90:E101,3,0)</f>
         <v>0.96</v>
       </c>
-      <c r="I94" s="101"/>
-      <c r="J94" s="101"/>
+      <c r="I94" s="93"/>
+      <c r="J94" s="93"/>
       <c r="K94">
         <f>VLOOKUP(G94,C90:E101,2,0)</f>
         <v>9</v>
@@ -9001,7 +8997,7 @@
         <v>0.76</v>
       </c>
       <c r="F95" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>PASS</v>
       </c>
     </row>
@@ -9019,7 +9015,7 @@
         <v>0.65</v>
       </c>
       <c r="F96" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -9037,7 +9033,7 @@
         <v>0.89</v>
       </c>
       <c r="F97" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>PASS</v>
       </c>
     </row>
@@ -9055,7 +9051,7 @@
         <v>0.88</v>
       </c>
       <c r="F98" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FAIL</v>
       </c>
     </row>
@@ -9073,7 +9069,7 @@
         <v>0.96</v>
       </c>
       <c r="F99" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FAIL</v>
       </c>
       <c r="H99" s="23" t="s">
@@ -9106,7 +9102,7 @@
         <v>0.9</v>
       </c>
       <c r="F100" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>PASS</v>
       </c>
       <c r="H100" s="23">
@@ -9139,7 +9135,7 @@
         <v>0.78</v>
       </c>
       <c r="F101" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FAIL</v>
       </c>
       <c r="H101" s="23">
@@ -9340,11 +9336,11 @@
         <v>1500</v>
       </c>
       <c r="E113" s="22">
-        <f t="shared" ref="E113:F123" si="7">VLOOKUP(I100,I99:M110,3,0)</f>
+        <f t="shared" ref="E113:F123" si="8">VLOOKUP(I100,I99:M110,3,0)</f>
         <v>2346</v>
       </c>
       <c r="F113" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>678</v>
       </c>
     </row>
@@ -9356,15 +9352,15 @@
         <v>104</v>
       </c>
       <c r="D114" s="22">
-        <f t="shared" ref="D114:D122" si="8">VLOOKUP(H101,H100:L111,3,0)</f>
+        <f t="shared" ref="D114:D122" si="9">VLOOKUP(H101,H100:L111,3,0)</f>
         <v>1200</v>
       </c>
       <c r="E114" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2345</v>
       </c>
       <c r="F114" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3455</v>
       </c>
     </row>
@@ -9376,15 +9372,15 @@
         <v>105</v>
       </c>
       <c r="D115" s="22">
+        <f t="shared" si="9"/>
+        <v>780</v>
+      </c>
+      <c r="E115" s="22">
         <f t="shared" si="8"/>
-        <v>780</v>
-      </c>
-      <c r="E115" s="22">
-        <f t="shared" si="7"/>
         <v>678</v>
       </c>
       <c r="F115" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6778</v>
       </c>
     </row>
@@ -9396,15 +9392,15 @@
         <v>106</v>
       </c>
       <c r="D116" s="22">
+        <f t="shared" si="9"/>
+        <v>908</v>
+      </c>
+      <c r="E116" s="22">
         <f t="shared" si="8"/>
-        <v>908</v>
-      </c>
-      <c r="E116" s="22">
-        <f t="shared" si="7"/>
         <v>897</v>
       </c>
       <c r="F116" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>678</v>
       </c>
     </row>
@@ -9416,15 +9412,15 @@
         <v>107</v>
       </c>
       <c r="D117" s="22">
+        <f t="shared" si="9"/>
+        <v>678</v>
+      </c>
+      <c r="E117" s="22">
         <f t="shared" si="8"/>
-        <v>678</v>
-      </c>
-      <c r="E117" s="22">
-        <f t="shared" si="7"/>
         <v>654</v>
       </c>
       <c r="F117" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>235</v>
       </c>
     </row>
@@ -9436,15 +9432,15 @@
         <v>108</v>
       </c>
       <c r="D118" s="22">
+        <f t="shared" si="9"/>
+        <v>675</v>
+      </c>
+      <c r="E118" s="22">
         <f t="shared" si="8"/>
-        <v>675</v>
-      </c>
-      <c r="E118" s="22">
-        <f t="shared" si="7"/>
         <v>345</v>
       </c>
       <c r="F118" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>567</v>
       </c>
     </row>
@@ -9456,15 +9452,15 @@
         <v>109</v>
       </c>
       <c r="D119" s="22">
+        <f t="shared" si="9"/>
+        <v>456</v>
+      </c>
+      <c r="E119" s="22">
         <f t="shared" si="8"/>
-        <v>456</v>
-      </c>
-      <c r="E119" s="22">
-        <f t="shared" si="7"/>
         <v>674</v>
       </c>
       <c r="F119" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>890</v>
       </c>
     </row>
@@ -9476,15 +9472,15 @@
         <v>110</v>
       </c>
       <c r="D120" s="22">
+        <f t="shared" si="9"/>
+        <v>234</v>
+      </c>
+      <c r="E120" s="22">
         <f t="shared" si="8"/>
-        <v>234</v>
-      </c>
-      <c r="E120" s="22">
-        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="F120" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>875</v>
       </c>
     </row>
@@ -9496,15 +9492,15 @@
         <v>114</v>
       </c>
       <c r="D121" s="22">
+        <f t="shared" si="9"/>
+        <v>567</v>
+      </c>
+      <c r="E121" s="22">
         <f t="shared" si="8"/>
-        <v>567</v>
-      </c>
-      <c r="E121" s="22">
-        <f t="shared" si="7"/>
         <v>809</v>
       </c>
       <c r="F121" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>326</v>
       </c>
     </row>
@@ -9516,15 +9512,15 @@
         <v>111</v>
       </c>
       <c r="D122" s="22">
+        <f t="shared" si="9"/>
+        <v>897</v>
+      </c>
+      <c r="E122" s="22">
         <f t="shared" si="8"/>
-        <v>897</v>
-      </c>
-      <c r="E122" s="22">
-        <f t="shared" si="7"/>
         <v>780</v>
       </c>
       <c r="F122" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>579</v>
       </c>
     </row>
@@ -9536,27 +9532,27 @@
         <v>111</v>
       </c>
       <c r="D123" s="22">
-        <f t="shared" ref="D123" si="9">VLOOKUP(H110,H109:L120,3,0)</f>
+        <f t="shared" ref="D123" si="10">VLOOKUP(H110,H109:L120,3,0)</f>
         <v>786</v>
       </c>
       <c r="E123" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>543</v>
       </c>
       <c r="F123" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1250</v>
       </c>
     </row>
     <row r="128" spans="2:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="E128" s="91" t="s">
+      <c r="E128" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="F128" s="91"/>
-      <c r="M128" s="92" t="s">
+      <c r="F128" s="83"/>
+      <c r="M128" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="N128" s="92"/>
+      <c r="N128" s="84"/>
     </row>
     <row r="131" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D131">
@@ -9728,12 +9724,12 @@
       </c>
     </row>
     <row r="149" spans="3:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="F149" s="93" t="s">
+      <c r="F149" s="85" t="s">
         <v>218</v>
       </c>
-      <c r="G149" s="93"/>
-      <c r="H149" s="93"/>
-      <c r="I149" s="93"/>
+      <c r="G149" s="85"/>
+      <c r="H149" s="85"/>
+      <c r="I149" s="85"/>
     </row>
     <row r="151" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C151" s="52" t="s">
@@ -11475,6 +11471,13 @@
     <sortCondition descending="1" ref="G151:G201"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="M4:O7"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:O25"/>
     <mergeCell ref="E128:F128"/>
     <mergeCell ref="M128:N128"/>
     <mergeCell ref="F149:I149"/>
@@ -11482,13 +11485,6 @@
     <mergeCell ref="J27:J31"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="H94:J94"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="M4:O7"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:O25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12090,10 +12086,10 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="K33" s="92"/>
-      <c r="L33" s="92"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="84"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="52" t="s">
@@ -13050,7 +13046,7 @@
   </sheetPr>
   <dimension ref="A2:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="56" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="56" workbookViewId="0">
       <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
@@ -15644,7 +15640,7 @@
   </sheetPr>
   <dimension ref="A3:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>

</xml_diff>